<commit_message>
Revert "Merge branch 'Tele-Mesmerism'"
This reverts commit 318aa9492112b4be7dd7eb38148982ade4b5e595, reversing
changes made to b7e2cc443cdfa9773cba7993a9ca260de3fcea43.
</commit_message>
<xml_diff>
--- a/documents/初步结构设计.xlsx
+++ b/documents/初步结构设计.xlsx
@@ -941,8 +941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="F37" workbookViewId="0">
+      <selection activeCell="H61" sqref="H61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>